<commit_message>
support mac & ip on host
</commit_message>
<xml_diff>
--- a/archon/resources/files/macip.xlsx
+++ b/archon/resources/files/macip.xlsx
@@ -399,7 +399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>